<commit_message>
ignore files are added
</commit_message>
<xml_diff>
--- a/Video Notes Excel.xlsx
+++ b/Video Notes Excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\furkan.altay\Documents\GitHub\desktop-tutorial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C812E71-7378-4E3E-A72C-E80610B1AEDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8CB9BA2-4087-4CBB-9566-1ACAD5A9E01B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7830" yWindow="-780" windowWidth="15450" windowHeight="11130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26220" yWindow="-825" windowWidth="15450" windowHeight="11130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>Sütun5</t>
   </si>
@@ -94,6 +94,15 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=2v_qM5SJDlY&amp;list=PLPW8O6W-1chwyTzI3BHwBLbGQoPFxPAPM&amp;index=13</t>
+  </si>
+  <si>
+    <t>Yok</t>
+  </si>
+  <si>
+    <t>What is the difference between array &amp; pointer array</t>
+  </si>
+  <si>
+    <t>yok</t>
   </si>
 </sst>
 </file>
@@ -555,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="F3:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="H7" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -690,10 +699,18 @@
       <c r="L10"/>
     </row>
     <row r="11" spans="6:12" ht="43.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
+      <c r="F11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="J11" s="2"/>
       <c r="K11"/>
       <c r="L11"/>

</xml_diff>